<commit_message>
made new times to avoid seizures
</commit_message>
<xml_diff>
--- a/data/seizure times.xlsx
+++ b/data/seizure times.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinconrad/Desktop/research/interictal_hubs/scripts/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF630A6-1C54-394D-97C3-9AA64F2418C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="1780" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="HUP99-complete" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="HUP100-complete" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="HUP110-complete" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="HUP111-complete" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="HUP128-complete" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="HUP132-complete" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="HUP136-complete-ish" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="HUP152-complete-ish" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="HUP193-complete" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="HUP201-complete" sheetId="10" r:id="rId13"/>
-    <sheet state="visible" name="HUP209-complete" sheetId="11" r:id="rId14"/>
-    <sheet state="visible" name="HUP168" sheetId="12" r:id="rId15"/>
-    <sheet state="visible" name="HUP101" sheetId="13" r:id="rId16"/>
+    <sheet name="HUP099-complete" sheetId="1" r:id="rId1"/>
+    <sheet name="HUP100-complete" sheetId="2" r:id="rId2"/>
+    <sheet name="HUP110-complete" sheetId="3" r:id="rId3"/>
+    <sheet name="HUP111-complete" sheetId="4" r:id="rId4"/>
+    <sheet name="HUP128-complete" sheetId="5" r:id="rId5"/>
+    <sheet name="HUP132-complete" sheetId="6" r:id="rId6"/>
+    <sheet name="HUP136-complete-ish" sheetId="7" r:id="rId7"/>
+    <sheet name="HUP152-complete-ish" sheetId="8" r:id="rId8"/>
+    <sheet name="HUP193-complete" sheetId="9" r:id="rId9"/>
+    <sheet name="HUP201-complete" sheetId="10" r:id="rId10"/>
+    <sheet name="HUP209-complete" sheetId="11" r:id="rId11"/>
+    <sheet name="HUP168" sheetId="12" r:id="rId12"/>
+    <sheet name="HUP101" sheetId="13" r:id="rId13"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -229,29 +238,34 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -261,87 +275,44 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -531,20 +502,23 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -570,38 +544,38 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1">
-        <v>9391.0</v>
+        <v>9391</v>
       </c>
       <c r="D2" s="1">
-        <v>9391.0</v>
+        <v>9391</v>
       </c>
       <c r="E2" s="1">
-        <v>9415.05</v>
+        <v>9415.0499999999993</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
-        <f t="shared" ref="A3:A19" si="1">A2+1</f>
+        <f t="shared" ref="A3:A19" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>10046.12</v>
+        <v>10046.120000000001</v>
       </c>
       <c r="D3" s="1">
-        <v>10046.12</v>
+        <v>10046.120000000001</v>
       </c>
       <c r="E3" s="1">
         <v>10067.18</v>
@@ -613,13 +587,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1">
         <v>10307.24</v>
@@ -637,19 +611,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>10415.03</v>
+        <v>10415.030000000001</v>
       </c>
       <c r="D5" s="1">
-        <v>10427.3</v>
+        <v>10427.299999999999</v>
       </c>
       <c r="E5" s="1">
         <v>10435.93</v>
@@ -661,13 +635,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>14135.52</v>
@@ -685,13 +659,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1">
         <v>228691.06</v>
@@ -709,19 +683,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1">
-        <v>229224.96</v>
+        <v>229224.95999999999</v>
       </c>
       <c r="D8" s="1">
-        <v>229224.96</v>
+        <v>229224.95999999999</v>
       </c>
       <c r="E8" s="1">
         <v>229268.85</v>
@@ -733,13 +707,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1">
         <v>230429.27</v>
@@ -757,13 +731,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1">
         <v>255274.69</v>
@@ -781,22 +755,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1">
-        <v>321466.04</v>
+        <v>321466.03999999998</v>
       </c>
       <c r="D11" s="1">
-        <v>321466.04</v>
+        <v>321466.03999999998</v>
       </c>
       <c r="E11" s="1">
-        <v>321482.96</v>
+        <v>321482.96000000002</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>8</v>
@@ -805,13 +779,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1">
         <v>322038.64</v>
@@ -829,13 +803,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C13" s="1">
         <v>336193.76</v>
@@ -853,13 +827,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1">
         <v>338048.68</v>
@@ -877,13 +851,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1">
         <v>374638.05</v>
@@ -901,13 +875,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C16" s="1">
         <v>521325.2</v>
@@ -922,13 +896,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1">
         <v>139903.46</v>
@@ -943,13 +917,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1">
         <v>160309.35</v>
@@ -964,13 +938,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1">
         <v>306080.49</v>
@@ -986,21 +960,22 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1026,12 +1001,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>89989.66</v>
@@ -1046,18 +1021,18 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>187555.0</v>
+        <v>187555</v>
       </c>
       <c r="D3" s="1">
-        <v>187555.0</v>
+        <v>187555</v>
       </c>
       <c r="E3" s="1">
         <v>187644.75</v>
@@ -1066,12 +1041,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
         <v>243441.45</v>
@@ -1086,12 +1061,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
         <v>231989.38</v>
@@ -1103,12 +1078,12 @@
         <v>232095.55</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
         <v>287840.98</v>
@@ -1123,12 +1098,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
         <v>487270.6</v>
@@ -1144,21 +1119,22 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1184,12 +1160,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="4">
         <v>224467.79</v>
@@ -1204,12 +1180,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="4">
         <v>236351.47</v>
@@ -1224,12 +1200,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="4">
         <v>255877.78</v>
@@ -1242,21 +1218,22 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1276,12 +1253,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>186009.3</v>
@@ -1296,12 +1273,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>216093.01</v>
@@ -1316,18 +1293,18 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>270894.46</v>
+        <v>270894.46000000002</v>
       </c>
       <c r="D4" s="1">
-        <v>270894.46</v>
+        <v>270894.46000000002</v>
       </c>
       <c r="E4" s="1">
         <v>270945.98</v>
@@ -1336,38 +1313,38 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>280484.22</v>
+        <v>280484.21999999997</v>
       </c>
       <c r="D5" s="1">
-        <v>280484.22</v>
+        <v>280484.21999999997</v>
       </c>
       <c r="E5" s="1">
-        <v>280547.96</v>
+        <v>280547.96000000002</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>308989.79</v>
+        <v>308989.78999999998</v>
       </c>
       <c r="D6" s="1">
-        <v>308989.79</v>
+        <v>308989.78999999998</v>
       </c>
       <c r="E6" s="1">
         <v>309008.01</v>
@@ -1376,12 +1353,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
         <v>203557.34</v>
@@ -1396,12 +1373,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1">
         <v>267733.94</v>
@@ -1416,12 +1393,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1">
         <v>383067.57</v>
@@ -1436,12 +1413,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1">
         <v>488897.46</v>
@@ -1457,21 +1434,22 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1497,21 +1475,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>514121.0</v>
+        <v>514121</v>
       </c>
       <c r="D2" s="1">
-        <v>514121.0</v>
+        <v>514121</v>
       </c>
       <c r="E2" s="1">
-        <v>514332.0</v>
+        <v>514332</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>63</v>
@@ -1520,122 +1498,123 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>525847.0</v>
+        <v>525847</v>
       </c>
       <c r="D3" s="1">
-        <v>525847.0</v>
+        <v>525847</v>
       </c>
       <c r="E3" s="1">
-        <v>525868.0</v>
+        <v>525868</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>554355.0</v>
+        <v>554355</v>
       </c>
       <c r="D4" s="1">
-        <v>554355.0</v>
+        <v>554355</v>
       </c>
       <c r="E4" s="1">
-        <v>554380.0</v>
+        <v>554380</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>581246.0</v>
+        <v>581246</v>
       </c>
       <c r="D5" s="1">
-        <v>581291.0</v>
+        <v>581291</v>
       </c>
       <c r="E5" s="1">
-        <v>581463.0</v>
+        <v>581463</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>590441.0</v>
+        <v>590441</v>
       </c>
       <c r="D6" s="1">
-        <v>590441.0</v>
+        <v>590441</v>
       </c>
       <c r="E6" s="1">
-        <v>590487.0</v>
+        <v>590487</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>704993.0</v>
+        <v>704993</v>
       </c>
       <c r="D7" s="1">
-        <v>704993.0</v>
+        <v>704993</v>
       </c>
       <c r="E7" s="1">
-        <v>705007.0</v>
+        <v>705007</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1661,12 +1640,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>8816.75</v>
@@ -1682,19 +1661,19 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
-        <f t="shared" ref="A3:A11" si="1">1+A2</f>
+        <f t="shared" ref="A3:A11" si="0">1+A2</f>
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>54591.2</v>
+        <v>54591.199999999997</v>
       </c>
       <c r="D3" s="1">
-        <v>54591.2</v>
+        <v>54591.199999999997</v>
       </c>
       <c r="E3" s="1">
         <v>54637.74</v>
@@ -1704,19 +1683,19 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>59253.0</v>
+        <v>59253</v>
       </c>
       <c r="D4" s="1">
-        <v>59253.0</v>
+        <v>59253</v>
       </c>
       <c r="E4" s="1">
         <v>59312.6</v>
@@ -1725,13 +1704,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
         <v>122854.47</v>
@@ -1746,13 +1725,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
         <v>150988.68</v>
@@ -1761,19 +1740,19 @@
         <v>150988.68</v>
       </c>
       <c r="E6" s="1">
-        <v>151059.3</v>
+        <v>151059.29999999999</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
         <v>229067.73</v>
@@ -1788,19 +1767,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>312096.0</v>
+        <v>312096</v>
       </c>
       <c r="D8" s="1">
-        <v>312096.0</v>
+        <v>312096</v>
       </c>
       <c r="E8" s="1">
         <v>312151.17</v>
@@ -1809,19 +1788,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>319255.0</v>
+        <v>319255</v>
       </c>
       <c r="D9" s="1">
-        <v>319255.0</v>
+        <v>319255</v>
       </c>
       <c r="E9" s="1">
         <v>319530.39</v>
@@ -1830,22 +1809,22 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>146397.0</v>
+        <v>146397</v>
       </c>
       <c r="D10" s="1">
-        <v>146413.0</v>
+        <v>146413</v>
       </c>
       <c r="E10" s="1">
-        <v>146503.0</v>
+        <v>146503</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>19</v>
@@ -1854,43 +1833,44 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1">
         <v>310047.05</v>
       </c>
       <c r="D11" s="1">
-        <v>310118.6</v>
+        <v>310118.59999999998</v>
       </c>
       <c r="E11" s="1">
-        <v>310206.0</v>
+        <v>310206</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1916,18 +1896,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>144677.55</v>
+        <v>144677.54999999999</v>
       </c>
       <c r="D2" s="1">
-        <v>144677.55</v>
+        <v>144677.54999999999</v>
       </c>
       <c r="E2" s="1">
         <v>144705.19</v>
@@ -1939,12 +1919,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>146788.47</v>
@@ -1962,18 +1942,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>147100.05</v>
+        <v>147100.04999999999</v>
       </c>
       <c r="D4" s="1">
-        <v>147100.05</v>
+        <v>147100.04999999999</v>
       </c>
       <c r="E4" s="1">
         <v>147117.47</v>
@@ -1985,18 +1965,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>147215.45</v>
+        <v>147215.45000000001</v>
       </c>
       <c r="D5" s="1">
-        <v>147215.45</v>
+        <v>147215.45000000001</v>
       </c>
       <c r="E5" s="1">
         <v>147227.43</v>
@@ -2008,18 +1988,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>147655.39</v>
+        <v>147655.39000000001</v>
       </c>
       <c r="D6" s="1">
-        <v>147655.39</v>
+        <v>147655.39000000001</v>
       </c>
       <c r="E6" s="1">
         <v>147671.32</v>
@@ -2031,21 +2011,21 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>148255.3</v>
+        <v>148255.29999999999</v>
       </c>
       <c r="D7" s="1">
-        <v>148255.3</v>
+        <v>148255.29999999999</v>
       </c>
       <c r="E7" s="1">
-        <v>148267.39</v>
+        <v>148267.39000000001</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>21</v>
@@ -2054,12 +2034,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
         <v>148255.12</v>
@@ -2068,7 +2048,7 @@
         <v>148255.12</v>
       </c>
       <c r="E8" s="1">
-        <v>148267.45</v>
+        <v>148267.45000000001</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>21</v>
@@ -2077,12 +2057,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1">
         <v>214605.04</v>
@@ -2100,12 +2080,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1">
         <v>224085.57</v>
@@ -2123,12 +2103,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1">
         <v>225995.79</v>
@@ -2146,12 +2126,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1">
         <v>231097.55</v>
@@ -2169,12 +2149,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1">
         <v>231665.46</v>
@@ -2192,12 +2172,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1">
         <v>232140.37</v>
@@ -2215,12 +2195,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1">
         <v>232849.31</v>
@@ -2238,12 +2218,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1">
         <v>236179.35</v>
@@ -2261,12 +2241,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1">
         <v>236832.54</v>
@@ -2284,12 +2264,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1">
         <v>249491.01</v>
@@ -2307,12 +2287,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1">
         <v>254677.21</v>
@@ -2330,12 +2310,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1">
         <v>255188.66</v>
@@ -2353,12 +2333,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="1">
         <v>265891.45</v>
@@ -2367,7 +2347,7 @@
         <v>265891.45</v>
       </c>
       <c r="E21" s="1">
-        <v>266033.53</v>
+        <v>266033.53000000003</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>24</v>
@@ -2376,12 +2356,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="1">
         <v>266199.93</v>
@@ -2399,12 +2379,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1">
         <v>266511.31</v>
@@ -2422,12 +2402,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="1">
         <v>267057.63</v>
@@ -2436,7 +2416,7 @@
         <v>267057.63</v>
       </c>
       <c r="E24" s="1">
-        <v>267200.16</v>
+        <v>267200.15999999997</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>24</v>
@@ -2445,21 +2425,21 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="1">
-        <v>334822.0</v>
+        <v>334822</v>
       </c>
       <c r="D25" s="1">
-        <v>334822.0</v>
+        <v>334822</v>
       </c>
       <c r="E25" s="1">
-        <v>334942.0</v>
+        <v>334942</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>24</v>
@@ -2468,12 +2448,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="1">
         <v>337638.77</v>
@@ -2491,18 +2471,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="1">
-        <v>339828.0</v>
+        <v>339828</v>
       </c>
       <c r="D27" s="1">
-        <v>339828.0</v>
+        <v>339828</v>
       </c>
       <c r="E27" s="1">
         <v>340130.76</v>
@@ -2514,12 +2494,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="1">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="1">
         <v>348259.71</v>
@@ -2537,12 +2517,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="1">
         <v>349798.76</v>
@@ -2560,12 +2540,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="1">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="1">
         <v>355052.47</v>
@@ -2583,12 +2563,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C31" s="1">
         <v>382548.96</v>
@@ -2606,12 +2586,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="1">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="1">
         <v>247327.95</v>
@@ -2629,25 +2609,26 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1000">
+    <row r="1000" spans="7:7" ht="13" x14ac:dyDescent="0.15">
       <c r="G1000" s="1"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2673,12 +2654,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>75640.38</v>
@@ -2693,12 +2674,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>130487.94</v>
@@ -2713,12 +2694,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
         <v>142718.88</v>
@@ -2727,24 +2708,24 @@
         <v>142718.88</v>
       </c>
       <c r="E4" s="1">
-        <v>142800.39</v>
+        <v>142800.39000000001</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>152116.92</v>
+        <v>152116.92000000001</v>
       </c>
       <c r="D5" s="1">
-        <v>152116.92</v>
+        <v>152116.92000000001</v>
       </c>
       <c r="E5" s="1">
         <v>152178.93</v>
@@ -2753,12 +2734,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
         <v>185739.31</v>
@@ -2773,29 +2754,29 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
-        <v>137727.98</v>
+        <v>137727.98000000001</v>
       </c>
       <c r="D7" s="1">
-        <v>137727.98</v>
+        <v>137727.98000000001</v>
       </c>
       <c r="E7" s="1">
-        <v>137737.08</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>137737.07999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1">
         <v>138590.84</v>
@@ -2804,15 +2785,15 @@
         <v>138590.84</v>
       </c>
       <c r="E8" s="1">
-        <v>138600.92</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>138600.92000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1">
         <v>161278.96</v>
@@ -2824,141 +2805,142 @@
         <v>161289.79</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>162630.0</v>
+        <v>162630</v>
       </c>
       <c r="D10" s="1">
-        <v>162630.0</v>
+        <v>162630</v>
       </c>
       <c r="E10" s="1">
-        <v>162639.23</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>162639.23000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1">
-        <v>167404.0</v>
+        <v>167404</v>
       </c>
       <c r="D11" s="1">
-        <v>167404.0</v>
+        <v>167404</v>
       </c>
       <c r="E11" s="1">
         <v>167411.53</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1">
-        <v>170938.0</v>
+        <v>170938</v>
       </c>
       <c r="D12" s="1">
-        <v>170938.0</v>
+        <v>170938</v>
       </c>
       <c r="E12" s="1">
         <v>171002.14</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C13" s="1">
-        <v>173585.0</v>
+        <v>173585</v>
       </c>
       <c r="D13" s="1">
-        <v>173585.0</v>
+        <v>173585</v>
       </c>
       <c r="E13" s="1">
         <v>173656.82</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1">
-        <v>175720.0</v>
+        <v>175720</v>
       </c>
       <c r="D14" s="1">
-        <v>175720.0</v>
+        <v>175720</v>
       </c>
       <c r="E14" s="1">
         <v>175796.05</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C15" s="1">
-        <v>220066.0</v>
+        <v>220066</v>
       </c>
       <c r="D15" s="1">
-        <v>220066.0</v>
+        <v>220066</v>
       </c>
       <c r="E15" s="1">
         <v>220129.22</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C16" s="1">
-        <v>222579.0</v>
+        <v>222579</v>
       </c>
       <c r="D16" s="1">
-        <v>222579.0</v>
+        <v>222579</v>
       </c>
       <c r="E16" s="1">
         <v>222665.09</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2984,12 +2966,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>394669.26</v>
@@ -3007,12 +2989,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>398915.81</v>
@@ -3030,12 +3012,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
         <v>645770.48</v>
@@ -3047,12 +3029,12 @@
         <v>645826.14</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
         <v>284420.12</v>
@@ -3061,18 +3043,18 @@
         <v>284420.12</v>
       </c>
       <c r="E5" s="1">
-        <v>284500.6</v>
+        <v>284500.59999999998</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
         <v>420557.57</v>
@@ -3081,28 +3063,29 @@
         <v>420557.57</v>
       </c>
       <c r="E6" s="1">
-        <v>420631.0</v>
+        <v>420631</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3128,15 +3111,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1">
-        <v>57516.0</v>
+        <v>57516</v>
       </c>
       <c r="E2" s="1">
         <v>57525.16</v>
@@ -3148,19 +3131,19 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
-        <f t="shared" ref="A3:A15" si="1">A2+1</f>
+        <f t="shared" ref="A3:A15" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>58894.0</v>
+        <v>58894</v>
       </c>
       <c r="D3" s="1">
-        <v>58894.0</v>
+        <v>58894</v>
       </c>
       <c r="E3" s="1">
         <v>58923.11</v>
@@ -3169,16 +3152,16 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>65463.0</v>
+        <v>65463</v>
       </c>
       <c r="E4" s="1">
         <v>65482.75</v>
@@ -3190,16 +3173,16 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>113163.0</v>
+        <v>113163</v>
       </c>
       <c r="D5" s="1">
         <v>113195.68</v>
@@ -3211,13 +3194,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
         <v>116629.25</v>
@@ -3226,37 +3209,37 @@
         <v>116629.25</v>
       </c>
       <c r="E6" s="1">
-        <v>116652.0</v>
+        <v>116652</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
-        <v>185043.0</v>
+        <v>185043</v>
       </c>
       <c r="E7" s="1">
-        <v>185103.0</v>
+        <v>185103</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1">
         <v>233586.3</v>
@@ -3271,13 +3254,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1">
         <v>249900.12</v>
@@ -3292,13 +3275,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1">
         <v>252713.73</v>
@@ -3313,13 +3296,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1">
         <v>265469.08</v>
@@ -3328,13 +3311,13 @@
         <v>265469.08</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1">
         <v>271404.13</v>
@@ -3343,43 +3326,43 @@
         <v>271404.13</v>
       </c>
       <c r="E12" s="1">
-        <v>271499.03</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>271499.03000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1">
-        <v>167111.98</v>
+        <v>167111.98000000001</v>
       </c>
       <c r="D13" s="1">
-        <v>167111.98</v>
+        <v>167111.98000000001</v>
       </c>
       <c r="E13" s="1">
-        <v>167138.8</v>
+        <v>167138.79999999999</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1">
-        <v>440685.0</v>
+        <v>440685</v>
       </c>
       <c r="D14" s="1">
-        <v>440685.0</v>
+        <v>440685</v>
       </c>
       <c r="E14" s="1">
         <v>440706.46</v>
@@ -3388,19 +3371,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1">
-        <v>441308.0</v>
+        <v>441308</v>
       </c>
       <c r="D15" s="1">
-        <v>441308.0</v>
+        <v>441308</v>
       </c>
       <c r="E15" s="1">
         <v>441351.32</v>
@@ -3410,21 +3393,22 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3450,23 +3434,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>309557.79</v>
+        <v>309557.78999999998</v>
       </c>
       <c r="D2" s="1">
-        <v>309557.79</v>
+        <v>309557.78999999998</v>
       </c>
       <c r="E2" s="1">
         <v>309595.76</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>314887.05</v>
@@ -3478,9 +3462,9 @@
         <v>314946.2</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
         <v>367035.29</v>
@@ -3492,9 +3476,9 @@
         <v>367106.17</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
         <v>422236.37</v>
@@ -3503,12 +3487,12 @@
         <v>422236.37</v>
       </c>
       <c r="E5" s="1">
-        <v>422670.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>422670</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
         <v>508463.62</v>
@@ -3520,9 +3504,9 @@
         <v>508525.87</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
         <v>510475.97</v>
@@ -3534,50 +3518,51 @@
         <v>510727.35</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1">
-        <v>530069.0</v>
+        <v>530069</v>
       </c>
       <c r="D8" s="1">
-        <v>530069.0</v>
+        <v>530069</v>
       </c>
       <c r="E8" s="1">
-        <v>530123.67</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>530123.67000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1">
-        <v>533815.81</v>
+        <v>533815.81000000006</v>
       </c>
       <c r="D9" s="1">
-        <v>533815.81</v>
+        <v>533815.81000000006</v>
       </c>
       <c r="E9" s="1">
-        <v>533920.45</v>
+        <v>533920.44999999995</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3603,9 +3588,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1">
         <v>313279.86</v>
@@ -3614,7 +3599,7 @@
         <v>313279.86</v>
       </c>
       <c r="E2" s="1">
-        <v>313353.79</v>
+        <v>313353.78999999998</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>37</v>
@@ -3623,9 +3608,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
         <v>380431.33</v>
@@ -3643,9 +3628,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>399709.29</v>
@@ -3663,9 +3648,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
         <v>418631.75</v>
@@ -3683,9 +3668,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
         <v>428511.13</v>
@@ -3703,9 +3688,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
         <v>438106.21</v>
@@ -3724,21 +3709,22 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3764,12 +3750,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>233763.21</v>
@@ -3787,13 +3773,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
-        <f t="shared" ref="A3:A11" si="1">A2+1</f>
+        <f t="shared" ref="A3:A11" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1">
         <v>72710.09</v>
@@ -3811,13 +3797,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>121240.28</v>
@@ -3835,19 +3821,19 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>145043.73</v>
+        <v>145043.73000000001</v>
       </c>
       <c r="D5" s="1">
-        <v>145051.2</v>
+        <v>145051.20000000001</v>
       </c>
       <c r="E5" s="1">
         <v>145174.18</v>
@@ -3859,13 +3845,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1">
         <v>23877.24</v>
@@ -3883,13 +3869,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1">
         <v>50816.03</v>
@@ -3907,13 +3893,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1">
         <v>87183.3</v>
@@ -3928,19 +3914,19 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1">
-        <v>108941.0</v>
+        <v>108941</v>
       </c>
       <c r="D9" s="1">
-        <v>108941.0</v>
+        <v>108941</v>
       </c>
       <c r="E9" s="1">
         <v>110203.65</v>
@@ -3952,22 +3938,22 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1">
-        <v>198387.0</v>
+        <v>198387</v>
       </c>
       <c r="D10" s="1">
-        <v>198387.0</v>
+        <v>198387</v>
       </c>
       <c r="E10" s="1">
-        <v>198558.0</v>
+        <v>198558</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>47</v>
@@ -3976,13 +3962,13 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1">
         <v>259244.64</v>
@@ -4001,6 +3987,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>